<commit_message>
RDM-2053 End Button Label Changes added
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V26_RDM-1473.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V26_RDM-1473.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fatiho/Documents/hmcts/workspace/case-definition-store-app/application/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fatiho/Documents/hmcts/workspace/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9314294E-091F-2D4A-9A32-3B8C3E205206}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28280" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28280" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -31,7 +32,7 @@
     <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId17"/>
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="275">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -869,6 +870,15 @@
   </si>
   <si>
     <t>Optional</t>
+  </si>
+  <si>
+    <t>EndButtonLabel</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Create Draft</t>
   </si>
 </sst>
 </file>
@@ -880,7 +890,7 @@
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1076,6 +1086,18 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1355,7 +1377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1527,6 +1549,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -15924,7 +15948,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -15975,7 +16001,7 @@
       <c r="O1" s="41"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
+      <c r="R1" s="120"/>
       <c r="S1" s="4"/>
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
@@ -16028,7 +16054,7 @@
       <c r="Q2" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="R2" s="5"/>
+      <c r="R2" s="123"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
@@ -16085,7 +16111,9 @@
       <c r="Q3" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="R3" s="8"/>
+      <c r="R3" s="124" t="s">
+        <v>272</v>
+      </c>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
       <c r="U3" s="8"/>
@@ -16126,7 +16154,9 @@
       <c r="Q4" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="R4" s="4"/>
+      <c r="R4" s="120" t="s">
+        <v>273</v>
+      </c>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
@@ -16169,7 +16199,9 @@
       <c r="Q5" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="R5" s="4"/>
+      <c r="R5" s="120" t="s">
+        <v>274</v>
+      </c>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
@@ -16212,7 +16244,7 @@
       <c r="Q6" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="R6" s="4"/>
+      <c r="R6" s="120"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
@@ -16253,7 +16285,7 @@
       <c r="Q7" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="R7" s="4"/>
+      <c r="R7" s="120"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
@@ -16296,7 +16328,7 @@
       <c r="Q8" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="R8" s="4"/>
+      <c r="R8" s="120"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
@@ -16337,7 +16369,7 @@
         <v>49</v>
       </c>
       <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="R9" s="120"/>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
@@ -16360,7 +16392,7 @@
       <c r="O10" s="41"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
+      <c r="R10" s="120"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
@@ -16383,7 +16415,7 @@
       <c r="O11" s="41"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="R11" s="120"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
@@ -16406,7 +16438,7 @@
       <c r="O12" s="41"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
+      <c r="R12" s="120"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
@@ -16429,7 +16461,7 @@
       <c r="O13" s="41"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
+      <c r="R13" s="120"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
@@ -16452,7 +16484,7 @@
       <c r="O14" s="41"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
+      <c r="R14" s="120"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
@@ -16475,7 +16507,7 @@
       <c r="O15" s="41"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
+      <c r="R15" s="120"/>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
@@ -16498,7 +16530,7 @@
       <c r="O16" s="41"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
+      <c r="R16" s="120"/>
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
@@ -16521,7 +16553,7 @@
       <c r="O17" s="41"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
+      <c r="R17" s="120"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
@@ -16544,7 +16576,7 @@
       <c r="O18" s="41"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
+      <c r="R18" s="120"/>
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
@@ -16567,7 +16599,7 @@
       <c r="O19" s="41"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
+      <c r="R19" s="120"/>
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
@@ -16585,7 +16617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>

</xml_diff>